<commit_message>
Worked on Card Class.
Added some methods to player and game to support card class.
</commit_message>
<xml_diff>
--- a/Monopoly Game .xlsx
+++ b/Monopoly Game .xlsx
@@ -5,15 +5,16 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adambailey/Dropbox/_GCC/_Classes/COMP 220 B/Project 4/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adambailey/Documents/localWorkspace/Project4-Monopoly/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="28800" windowHeight="16580" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="40" yWindow="440" windowWidth="28800" windowHeight="16580" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Classes" sheetId="1" r:id="rId1"/>
     <sheet name="Properties" sheetId="2" r:id="rId2"/>
+    <sheet name="Cards" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="151">
   <si>
     <t>Player</t>
   </si>
@@ -349,6 +350,138 @@
   </si>
   <si>
     <t>Residential</t>
+  </si>
+  <si>
+    <t>CHANCE:</t>
+  </si>
+  <si>
+    <t>Title</t>
+  </si>
+  <si>
+    <t>moveTo</t>
+  </si>
+  <si>
+    <t>fine</t>
+  </si>
+  <si>
+    <t>get</t>
+  </si>
+  <si>
+    <t>Advance to Go</t>
+  </si>
+  <si>
+    <t>Advance to Illinois Ave</t>
+  </si>
+  <si>
+    <t>Advance to St. Charles Place</t>
+  </si>
+  <si>
+    <t>Advance to Nearest RR</t>
+  </si>
+  <si>
+    <t>Bank Pays you $50</t>
+  </si>
+  <si>
+    <t>Get Out of Jail Free</t>
+  </si>
+  <si>
+    <t>SPECIAL</t>
+  </si>
+  <si>
+    <t>SPECIAL #</t>
+  </si>
+  <si>
+    <t>Go back three spaces</t>
+  </si>
+  <si>
+    <t>notes</t>
+  </si>
+  <si>
+    <t>pos - 3</t>
+  </si>
+  <si>
+    <t>Go To Jail, Go Directly To Jail</t>
+  </si>
+  <si>
+    <t>pos = 10</t>
+  </si>
+  <si>
+    <t>Make Repairs to Properties</t>
+  </si>
+  <si>
+    <t>house = -$25, hotel = -$100</t>
+  </si>
+  <si>
+    <t>Pay Poor Tax</t>
+  </si>
+  <si>
+    <t>Take a Trip on the Reading RR</t>
+  </si>
+  <si>
+    <t>pos = 5</t>
+  </si>
+  <si>
+    <t>Take a Walk on the Boardwalk</t>
+  </si>
+  <si>
+    <t>pay each player $50</t>
+  </si>
+  <si>
+    <t>Your Building and Loan Matures</t>
+  </si>
+  <si>
+    <t>You've Been Elected Chairman of the Board</t>
+  </si>
+  <si>
+    <t>Bank Error in Your Favor</t>
+  </si>
+  <si>
+    <t>Doctor's Fees</t>
+  </si>
+  <si>
+    <t>From Sale of Stock You Get $50</t>
+  </si>
+  <si>
+    <t>Grand Opera Night</t>
+  </si>
+  <si>
+    <t>collect $50 from each player</t>
+  </si>
+  <si>
+    <t>Holiday Fund Matures</t>
+  </si>
+  <si>
+    <t>Income Tax Refund</t>
+  </si>
+  <si>
+    <t>It's Your Birthday</t>
+  </si>
+  <si>
+    <t>$10 from each player</t>
+  </si>
+  <si>
+    <t>Life Insurance Matures</t>
+  </si>
+  <si>
+    <t>Pay Hostpital Fees</t>
+  </si>
+  <si>
+    <t>Pay School Fees</t>
+  </si>
+  <si>
+    <t>Receive $25 Consultancy Fee</t>
+  </si>
+  <si>
+    <t>You Are Assessed for Street Pairs</t>
+  </si>
+  <si>
+    <t>$40 per house, $115 per hotel</t>
+  </si>
+  <si>
+    <t>You Have Won Second Prize in a Beauty Contest</t>
+  </si>
+  <si>
+    <t>You Inherit $100</t>
   </si>
 </sst>
 </file>
@@ -358,7 +491,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -435,8 +568,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="25">
+  <fills count="27">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -579,6 +719,18 @@
       <patternFill patternType="solid">
         <fgColor theme="5" tint="-0.499984740745262"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF000000"/>
+        <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
   </fills>
@@ -807,7 +959,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="9">
+  <cellStyleXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -817,8 +969,10 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="80">
+  <cellXfs count="82">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -916,6 +1070,10 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="22" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="23" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="164" fontId="5" fillId="19" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -925,20 +1083,20 @@
     <xf numFmtId="164" fontId="5" fillId="19" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="9">
+  <cellStyles count="11">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1685,7 +1843,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A3" workbookViewId="0">
       <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
@@ -1701,44 +1859,44 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" s="57" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="76" t="s">
+      <c r="A1" s="78" t="s">
         <v>58</v>
       </c>
-      <c r="B1" s="76" t="s">
+      <c r="B1" s="78" t="s">
         <v>59</v>
       </c>
-      <c r="C1" s="76" t="s">
+      <c r="C1" s="78" t="s">
         <v>84</v>
       </c>
-      <c r="D1" s="76" t="s">
+      <c r="D1" s="78" t="s">
         <v>40</v>
       </c>
-      <c r="E1" s="77" t="s">
+      <c r="E1" s="79" t="s">
         <v>60</v>
       </c>
-      <c r="F1" s="77" t="s">
+      <c r="F1" s="79" t="s">
         <v>61</v>
       </c>
-      <c r="G1" s="77" t="s">
+      <c r="G1" s="79" t="s">
         <v>85</v>
       </c>
-      <c r="H1" s="75" t="s">
+      <c r="H1" s="77" t="s">
         <v>12</v>
       </c>
-      <c r="I1" s="75"/>
-      <c r="J1" s="75"/>
-      <c r="K1" s="75"/>
-      <c r="L1" s="75"/>
-      <c r="M1" s="75"/>
+      <c r="I1" s="77"/>
+      <c r="J1" s="77"/>
+      <c r="K1" s="77"/>
+      <c r="L1" s="77"/>
+      <c r="M1" s="77"/>
     </row>
     <row r="2" spans="1:13" s="59" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="76"/>
-      <c r="B2" s="76"/>
-      <c r="C2" s="76"/>
-      <c r="D2" s="76"/>
-      <c r="E2" s="77"/>
-      <c r="F2" s="77"/>
-      <c r="G2" s="77"/>
+      <c r="A2" s="78"/>
+      <c r="B2" s="78"/>
+      <c r="C2" s="78"/>
+      <c r="D2" s="78"/>
+      <c r="E2" s="79"/>
+      <c r="F2" s="79"/>
+      <c r="G2" s="79"/>
       <c r="H2" s="58" t="s">
         <v>86</v>
       </c>
@@ -1767,10 +1925,10 @@
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A4" s="78" t="s">
+      <c r="A4" s="75" t="s">
         <v>62</v>
       </c>
-      <c r="B4" s="79">
+      <c r="B4" s="76">
         <v>1</v>
       </c>
       <c r="C4" s="46">
@@ -1813,10 +1971,10 @@
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A6" s="78" t="s">
+      <c r="A6" s="75" t="s">
         <v>63</v>
       </c>
-      <c r="B6" s="79">
+      <c r="B6" s="76">
         <v>1</v>
       </c>
       <c r="C6" s="46">
@@ -2780,4 +2938,669 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G37"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="40.83203125" customWidth="1"/>
+    <col min="7" max="7" width="26" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" s="81" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" s="80" t="s">
+        <v>108</v>
+      </c>
+      <c r="B2" s="80" t="s">
+        <v>109</v>
+      </c>
+      <c r="C2" s="80" t="s">
+        <v>110</v>
+      </c>
+      <c r="D2" s="80" t="s">
+        <v>111</v>
+      </c>
+      <c r="E2" s="80" t="s">
+        <v>118</v>
+      </c>
+      <c r="F2" s="80" t="s">
+        <v>119</v>
+      </c>
+      <c r="G2" s="80" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>112</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>-1</v>
+      </c>
+      <c r="D3">
+        <v>-1</v>
+      </c>
+      <c r="E3" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>113</v>
+      </c>
+      <c r="B4">
+        <v>24</v>
+      </c>
+      <c r="C4">
+        <v>-1</v>
+      </c>
+      <c r="D4">
+        <v>-1</v>
+      </c>
+      <c r="E4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>114</v>
+      </c>
+      <c r="B5">
+        <v>11</v>
+      </c>
+      <c r="C5">
+        <v>-1</v>
+      </c>
+      <c r="D5">
+        <v>-1</v>
+      </c>
+      <c r="E5" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>115</v>
+      </c>
+      <c r="B6">
+        <v>-1</v>
+      </c>
+      <c r="C6">
+        <v>-1</v>
+      </c>
+      <c r="D6">
+        <v>-1</v>
+      </c>
+      <c r="E6" t="b">
+        <v>1</v>
+      </c>
+      <c r="F6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>116</v>
+      </c>
+      <c r="B7">
+        <v>-1</v>
+      </c>
+      <c r="C7">
+        <v>-1</v>
+      </c>
+      <c r="D7">
+        <v>50</v>
+      </c>
+      <c r="E7" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>117</v>
+      </c>
+      <c r="B8">
+        <v>-1</v>
+      </c>
+      <c r="C8">
+        <v>-1</v>
+      </c>
+      <c r="D8">
+        <v>-1</v>
+      </c>
+      <c r="E8" t="b">
+        <v>1</v>
+      </c>
+      <c r="F8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>120</v>
+      </c>
+      <c r="B9">
+        <v>-1</v>
+      </c>
+      <c r="C9">
+        <v>-1</v>
+      </c>
+      <c r="D9">
+        <v>-1</v>
+      </c>
+      <c r="E9" t="b">
+        <v>1</v>
+      </c>
+      <c r="F9">
+        <v>3</v>
+      </c>
+      <c r="G9" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>123</v>
+      </c>
+      <c r="B10">
+        <v>-1</v>
+      </c>
+      <c r="C10">
+        <v>-1</v>
+      </c>
+      <c r="D10">
+        <v>-1</v>
+      </c>
+      <c r="E10" t="b">
+        <v>1</v>
+      </c>
+      <c r="F10">
+        <v>4</v>
+      </c>
+      <c r="G10" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>125</v>
+      </c>
+      <c r="B11">
+        <v>-1</v>
+      </c>
+      <c r="C11">
+        <v>-1</v>
+      </c>
+      <c r="D11">
+        <v>-1</v>
+      </c>
+      <c r="E11" t="b">
+        <v>1</v>
+      </c>
+      <c r="F11">
+        <v>5</v>
+      </c>
+      <c r="G11" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>127</v>
+      </c>
+      <c r="B12">
+        <v>-1</v>
+      </c>
+      <c r="C12">
+        <v>15</v>
+      </c>
+      <c r="D12">
+        <v>-1</v>
+      </c>
+      <c r="E12" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>128</v>
+      </c>
+      <c r="B13">
+        <v>-1</v>
+      </c>
+      <c r="C13">
+        <v>-1</v>
+      </c>
+      <c r="D13">
+        <v>-1</v>
+      </c>
+      <c r="E13" t="b">
+        <v>1</v>
+      </c>
+      <c r="F13">
+        <v>6</v>
+      </c>
+      <c r="G13" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>130</v>
+      </c>
+      <c r="B14">
+        <v>39</v>
+      </c>
+      <c r="C14">
+        <v>-1</v>
+      </c>
+      <c r="D14">
+        <v>-1</v>
+      </c>
+      <c r="E14" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>133</v>
+      </c>
+      <c r="B15">
+        <v>-1</v>
+      </c>
+      <c r="C15">
+        <v>-1</v>
+      </c>
+      <c r="D15">
+        <v>-1</v>
+      </c>
+      <c r="E15" t="b">
+        <v>1</v>
+      </c>
+      <c r="F15">
+        <v>7</v>
+      </c>
+      <c r="G15" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>132</v>
+      </c>
+      <c r="B16">
+        <v>-1</v>
+      </c>
+      <c r="C16">
+        <v>-1</v>
+      </c>
+      <c r="D16">
+        <v>150</v>
+      </c>
+      <c r="E16" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A19" s="81" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A20" s="80" t="s">
+        <v>108</v>
+      </c>
+      <c r="B20" s="80" t="s">
+        <v>109</v>
+      </c>
+      <c r="C20" s="80" t="s">
+        <v>110</v>
+      </c>
+      <c r="D20" s="80" t="s">
+        <v>111</v>
+      </c>
+      <c r="E20" s="80" t="s">
+        <v>118</v>
+      </c>
+      <c r="F20" s="80" t="s">
+        <v>119</v>
+      </c>
+      <c r="G20" s="80" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>112</v>
+      </c>
+      <c r="B21">
+        <v>0</v>
+      </c>
+      <c r="C21">
+        <v>-1</v>
+      </c>
+      <c r="D21">
+        <v>-1</v>
+      </c>
+      <c r="E21" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>134</v>
+      </c>
+      <c r="B22">
+        <v>-1</v>
+      </c>
+      <c r="C22">
+        <v>-1</v>
+      </c>
+      <c r="D22">
+        <v>200</v>
+      </c>
+      <c r="E22" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>135</v>
+      </c>
+      <c r="B23">
+        <v>-1</v>
+      </c>
+      <c r="C23">
+        <v>50</v>
+      </c>
+      <c r="D23">
+        <v>-1</v>
+      </c>
+      <c r="E23" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>136</v>
+      </c>
+      <c r="B24">
+        <v>-1</v>
+      </c>
+      <c r="C24">
+        <v>-1</v>
+      </c>
+      <c r="D24">
+        <v>50</v>
+      </c>
+      <c r="E24" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>117</v>
+      </c>
+      <c r="B25">
+        <v>-1</v>
+      </c>
+      <c r="C25">
+        <v>-1</v>
+      </c>
+      <c r="D25">
+        <v>-1</v>
+      </c>
+      <c r="E25" t="b">
+        <v>1</v>
+      </c>
+      <c r="F25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>123</v>
+      </c>
+      <c r="B26">
+        <v>-1</v>
+      </c>
+      <c r="C26">
+        <v>-1</v>
+      </c>
+      <c r="D26">
+        <v>-1</v>
+      </c>
+      <c r="E26" t="b">
+        <v>1</v>
+      </c>
+      <c r="F26">
+        <v>2</v>
+      </c>
+      <c r="G26" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>137</v>
+      </c>
+      <c r="B27">
+        <v>-1</v>
+      </c>
+      <c r="C27">
+        <v>-1</v>
+      </c>
+      <c r="D27">
+        <v>-1</v>
+      </c>
+      <c r="E27" t="b">
+        <v>1</v>
+      </c>
+      <c r="F27">
+        <v>3</v>
+      </c>
+      <c r="G27" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>139</v>
+      </c>
+      <c r="B28">
+        <v>-1</v>
+      </c>
+      <c r="C28">
+        <v>-1</v>
+      </c>
+      <c r="D28">
+        <v>100</v>
+      </c>
+      <c r="E28" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>140</v>
+      </c>
+      <c r="B29">
+        <v>-1</v>
+      </c>
+      <c r="C29">
+        <v>-1</v>
+      </c>
+      <c r="D29">
+        <v>20</v>
+      </c>
+      <c r="E29" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>141</v>
+      </c>
+      <c r="B30">
+        <v>-1</v>
+      </c>
+      <c r="C30">
+        <v>-1</v>
+      </c>
+      <c r="D30">
+        <v>-1</v>
+      </c>
+      <c r="E30" t="b">
+        <v>1</v>
+      </c>
+      <c r="F30">
+        <v>4</v>
+      </c>
+      <c r="G30" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>143</v>
+      </c>
+      <c r="B31">
+        <v>-1</v>
+      </c>
+      <c r="C31">
+        <v>-1</v>
+      </c>
+      <c r="D31">
+        <v>100</v>
+      </c>
+      <c r="E31" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>144</v>
+      </c>
+      <c r="B32">
+        <v>-1</v>
+      </c>
+      <c r="C32">
+        <v>100</v>
+      </c>
+      <c r="D32">
+        <v>-1</v>
+      </c>
+      <c r="E32" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>145</v>
+      </c>
+      <c r="B33">
+        <v>-1</v>
+      </c>
+      <c r="C33">
+        <v>150</v>
+      </c>
+      <c r="D33">
+        <v>-1</v>
+      </c>
+      <c r="E33" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>146</v>
+      </c>
+      <c r="B34">
+        <v>-1</v>
+      </c>
+      <c r="C34">
+        <v>-1</v>
+      </c>
+      <c r="D34">
+        <v>25</v>
+      </c>
+      <c r="E34" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>147</v>
+      </c>
+      <c r="B35">
+        <v>-1</v>
+      </c>
+      <c r="C35">
+        <v>-1</v>
+      </c>
+      <c r="D35">
+        <v>-1</v>
+      </c>
+      <c r="E35" t="b">
+        <v>1</v>
+      </c>
+      <c r="F35">
+        <v>5</v>
+      </c>
+      <c r="G35" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>149</v>
+      </c>
+      <c r="B36">
+        <v>-1</v>
+      </c>
+      <c r="C36">
+        <v>-1</v>
+      </c>
+      <c r="D36">
+        <v>10</v>
+      </c>
+      <c r="E36" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>150</v>
+      </c>
+      <c r="B37">
+        <v>-1</v>
+      </c>
+      <c r="C37">
+        <v>-1</v>
+      </c>
+      <c r="D37">
+        <v>100</v>
+      </c>
+      <c r="E37" t="b">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Continued working on Chance Cards and supporting methods
</commit_message>
<xml_diff>
--- a/Monopoly Game .xlsx
+++ b/Monopoly Game .xlsx
@@ -9,12 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="40" yWindow="440" windowWidth="28800" windowHeight="16580" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="28800" windowHeight="16580" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Classes" sheetId="1" r:id="rId1"/>
     <sheet name="Properties" sheetId="2" r:id="rId2"/>
     <sheet name="Cards" sheetId="3" r:id="rId3"/>
+    <sheet name="To Do" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="168">
   <si>
     <t>Player</t>
   </si>
@@ -482,6 +483,57 @@
   </si>
   <si>
     <t>You Inherit $100</t>
+  </si>
+  <si>
+    <t>ACTION SPOT</t>
+  </si>
+  <si>
+    <t>CARD</t>
+  </si>
+  <si>
+    <t>CHANCE CARD</t>
+  </si>
+  <si>
+    <t>GAME</t>
+  </si>
+  <si>
+    <t>LOCATION</t>
+  </si>
+  <si>
+    <t>MAIN</t>
+  </si>
+  <si>
+    <t>PLAYER</t>
+  </si>
+  <si>
+    <t>PROPERTY</t>
+  </si>
+  <si>
+    <t>RESIDENTIAL</t>
+  </si>
+  <si>
+    <t>TAX</t>
+  </si>
+  <si>
+    <t>UTILITY</t>
+  </si>
+  <si>
+    <t>The whole thing</t>
+  </si>
+  <si>
+    <t>Constructor</t>
+  </si>
+  <si>
+    <t>cardAction()</t>
+  </si>
+  <si>
+    <t>rollDice()</t>
+  </si>
+  <si>
+    <t>mortgageProperties()</t>
+  </si>
+  <si>
+    <t>moveTo()</t>
   </si>
 </sst>
 </file>
@@ -491,7 +543,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0"/>
   </numFmts>
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -575,8 +627,36 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="27">
+  <fills count="30">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -730,6 +810,24 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF000000"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC00000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
         <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
@@ -959,7 +1057,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="11">
+  <cellStyleXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -971,8 +1069,10 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="82">
+  <cellXfs count="88">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -1074,6 +1174,8 @@
     <xf numFmtId="0" fontId="2" fillId="24" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="164" fontId="5" fillId="19" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1083,20 +1185,26 @@
     <xf numFmtId="164" fontId="5" fillId="19" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="11" fillId="25" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="27" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="13" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="14" fillId="28" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="14" fillId="29" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="11">
+  <cellStyles count="13">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1843,8 +1951,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M42"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+    <sheetView topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1859,44 +1967,44 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" s="57" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="78" t="s">
+      <c r="A1" s="80" t="s">
         <v>58</v>
       </c>
-      <c r="B1" s="78" t="s">
+      <c r="B1" s="80" t="s">
         <v>59</v>
       </c>
-      <c r="C1" s="78" t="s">
+      <c r="C1" s="80" t="s">
         <v>84</v>
       </c>
-      <c r="D1" s="78" t="s">
+      <c r="D1" s="80" t="s">
         <v>40</v>
       </c>
-      <c r="E1" s="79" t="s">
+      <c r="E1" s="81" t="s">
         <v>60</v>
       </c>
-      <c r="F1" s="79" t="s">
+      <c r="F1" s="81" t="s">
         <v>61</v>
       </c>
-      <c r="G1" s="79" t="s">
+      <c r="G1" s="81" t="s">
         <v>85</v>
       </c>
-      <c r="H1" s="77" t="s">
+      <c r="H1" s="79" t="s">
         <v>12</v>
       </c>
-      <c r="I1" s="77"/>
-      <c r="J1" s="77"/>
-      <c r="K1" s="77"/>
-      <c r="L1" s="77"/>
-      <c r="M1" s="77"/>
+      <c r="I1" s="79"/>
+      <c r="J1" s="79"/>
+      <c r="K1" s="79"/>
+      <c r="L1" s="79"/>
+      <c r="M1" s="79"/>
     </row>
     <row r="2" spans="1:13" s="59" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="78"/>
-      <c r="B2" s="78"/>
-      <c r="C2" s="78"/>
-      <c r="D2" s="78"/>
-      <c r="E2" s="79"/>
-      <c r="F2" s="79"/>
-      <c r="G2" s="79"/>
+      <c r="A2" s="80"/>
+      <c r="B2" s="80"/>
+      <c r="C2" s="80"/>
+      <c r="D2" s="80"/>
+      <c r="E2" s="81"/>
+      <c r="F2" s="81"/>
+      <c r="G2" s="81"/>
       <c r="H2" s="58" t="s">
         <v>86</v>
       </c>
@@ -2944,8 +3052,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2955,30 +3063,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1" s="81" t="s">
+      <c r="A1" s="78" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" s="80" t="s">
+      <c r="A2" s="77" t="s">
         <v>108</v>
       </c>
-      <c r="B2" s="80" t="s">
+      <c r="B2" s="77" t="s">
         <v>109</v>
       </c>
-      <c r="C2" s="80" t="s">
+      <c r="C2" s="77" t="s">
         <v>110</v>
       </c>
-      <c r="D2" s="80" t="s">
+      <c r="D2" s="77" t="s">
         <v>111</v>
       </c>
-      <c r="E2" s="80" t="s">
+      <c r="E2" s="77" t="s">
         <v>118</v>
       </c>
-      <c r="F2" s="80" t="s">
+      <c r="F2" s="77" t="s">
         <v>119</v>
       </c>
-      <c r="G2" s="80" t="s">
+      <c r="G2" s="77" t="s">
         <v>121</v>
       </c>
     </row>
@@ -3257,30 +3365,30 @@
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A19" s="81" t="s">
+      <c r="A19" s="78" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A20" s="80" t="s">
+      <c r="A20" s="77" t="s">
         <v>108</v>
       </c>
-      <c r="B20" s="80" t="s">
+      <c r="B20" s="77" t="s">
         <v>109</v>
       </c>
-      <c r="C20" s="80" t="s">
+      <c r="C20" s="77" t="s">
         <v>110</v>
       </c>
-      <c r="D20" s="80" t="s">
+      <c r="D20" s="77" t="s">
         <v>111</v>
       </c>
-      <c r="E20" s="80" t="s">
+      <c r="E20" s="77" t="s">
         <v>118</v>
       </c>
-      <c r="F20" s="80" t="s">
+      <c r="F20" s="77" t="s">
         <v>119</v>
       </c>
-      <c r="G20" s="80" t="s">
+      <c r="G20" s="77" t="s">
         <v>121</v>
       </c>
     </row>
@@ -3598,6 +3706,125 @@
       </c>
       <c r="E37" t="b">
         <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A66"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="A32" sqref="A32"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="40.83203125" style="83" customWidth="1"/>
+    <col min="2" max="16384" width="10.83203125" style="83"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" s="82" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="82" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" s="84" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" s="82" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="82" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" s="85" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" s="82" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="82" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14" s="85" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A15" s="86" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" s="82" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="82" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" s="85" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" s="86" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" s="87" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" s="87" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" s="82" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="82" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A32" s="85" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" s="82" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="82" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" s="82" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="82" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" s="82" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="82" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" s="82" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="82" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" s="82" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="82" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" s="82" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A66" s="82" t="s">
+        <v>161</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Began working through processing gameplay through UI.
</commit_message>
<xml_diff>
--- a/Monopoly Game .xlsx
+++ b/Monopoly Game .xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="28800" windowHeight="16580" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="28800" windowHeight="16580" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Classes" sheetId="1" r:id="rId1"/>
@@ -1488,7 +1488,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="M3" sqref="M3"/>
     </sheetView>
   </sheetViews>
@@ -1951,7 +1951,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M42"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
@@ -3717,8 +3717,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="A32" sqref="A32"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Worked on Dice Roll
</commit_message>
<xml_diff>
--- a/Monopoly Game .xlsx
+++ b/Monopoly Game .xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="28800" windowHeight="16580" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="28800" windowHeight="16580" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Classes" sheetId="1" r:id="rId1"/>
@@ -1488,7 +1488,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="M3" sqref="M3"/>
     </sheetView>
   </sheetViews>
@@ -3052,8 +3052,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Worked on Game method to create cards.
</commit_message>
<xml_diff>
--- a/Monopoly Game .xlsx
+++ b/Monopoly Game .xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="28800" windowHeight="16580" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="28800" windowHeight="16580" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Classes" sheetId="1" r:id="rId1"/>
@@ -1176,6 +1176,12 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="26" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="25" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="11" fillId="25" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="27" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="13" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="14" fillId="28" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="14" fillId="29" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="164" fontId="5" fillId="19" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1185,12 +1191,6 @@
     <xf numFmtId="164" fontId="5" fillId="19" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="25" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="13" fillId="27" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="13" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="14" fillId="28" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="14" fillId="29" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="13">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -1951,8 +1951,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M42"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1967,44 +1967,44 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" s="57" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="80" t="s">
+      <c r="A1" s="86" t="s">
         <v>58</v>
       </c>
-      <c r="B1" s="80" t="s">
+      <c r="B1" s="86" t="s">
         <v>59</v>
       </c>
-      <c r="C1" s="80" t="s">
+      <c r="C1" s="86" t="s">
         <v>84</v>
       </c>
-      <c r="D1" s="80" t="s">
+      <c r="D1" s="86" t="s">
         <v>40</v>
       </c>
-      <c r="E1" s="81" t="s">
+      <c r="E1" s="87" t="s">
         <v>60</v>
       </c>
-      <c r="F1" s="81" t="s">
+      <c r="F1" s="87" t="s">
         <v>61</v>
       </c>
-      <c r="G1" s="81" t="s">
+      <c r="G1" s="87" t="s">
         <v>85</v>
       </c>
-      <c r="H1" s="79" t="s">
+      <c r="H1" s="85" t="s">
         <v>12</v>
       </c>
-      <c r="I1" s="79"/>
-      <c r="J1" s="79"/>
-      <c r="K1" s="79"/>
-      <c r="L1" s="79"/>
-      <c r="M1" s="79"/>
+      <c r="I1" s="85"/>
+      <c r="J1" s="85"/>
+      <c r="K1" s="85"/>
+      <c r="L1" s="85"/>
+      <c r="M1" s="85"/>
     </row>
     <row r="2" spans="1:13" s="59" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="80"/>
-      <c r="B2" s="80"/>
-      <c r="C2" s="80"/>
-      <c r="D2" s="80"/>
-      <c r="E2" s="81"/>
-      <c r="F2" s="81"/>
-      <c r="G2" s="81"/>
+      <c r="A2" s="86"/>
+      <c r="B2" s="86"/>
+      <c r="C2" s="86"/>
+      <c r="D2" s="86"/>
+      <c r="E2" s="87"/>
+      <c r="F2" s="87"/>
+      <c r="G2" s="87"/>
       <c r="H2" s="58" t="s">
         <v>86</v>
       </c>
@@ -3052,7 +3052,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
@@ -3723,107 +3723,107 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="40.83203125" style="83" customWidth="1"/>
-    <col min="2" max="16384" width="10.83203125" style="83"/>
+    <col min="1" max="1" width="40.83203125" style="80" customWidth="1"/>
+    <col min="2" max="16384" width="10.83203125" style="80"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" s="82" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="82" t="s">
+    <row r="1" spans="1:1" s="79" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="79" t="s">
         <v>151</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" s="84" t="s">
+      <c r="A2" s="81" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="7" spans="1:1" s="82" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="82" t="s">
+    <row r="7" spans="1:1" s="79" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="79" t="s">
         <v>152</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A8" s="85" t="s">
+      <c r="A8" s="82" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="13" spans="1:1" s="82" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="82" t="s">
+    <row r="13" spans="1:1" s="79" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="79" t="s">
         <v>153</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A14" s="85" t="s">
+      <c r="A14" s="82" t="s">
         <v>163</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A15" s="86" t="s">
+      <c r="A15" s="83" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="19" spans="1:1" s="82" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="82" t="s">
+    <row r="19" spans="1:1" s="79" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="79" t="s">
         <v>154</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20" s="85" t="s">
+      <c r="A20" s="82" t="s">
         <v>163</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A21" s="86" t="s">
+      <c r="A21" s="83" t="s">
         <v>165</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A22" s="87" t="s">
+      <c r="A22" s="84" t="s">
         <v>166</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A23" s="87" t="s">
+      <c r="A23" s="84" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="31" spans="1:1" s="82" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="82" t="s">
+    <row r="31" spans="1:1" s="79" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="79" t="s">
         <v>155</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A32" s="85" t="s">
+      <c r="A32" s="82" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="37" spans="1:1" s="82" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="82" t="s">
+    <row r="37" spans="1:1" s="79" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="79" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="42" spans="1:1" s="82" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="82" t="s">
+    <row r="42" spans="1:1" s="79" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="79" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="48" spans="1:1" s="82" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="82" t="s">
+    <row r="48" spans="1:1" s="79" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="79" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="54" spans="1:1" s="82" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="82" t="s">
+    <row r="54" spans="1:1" s="79" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="79" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="60" spans="1:1" s="82" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="82" t="s">
+    <row r="60" spans="1:1" s="79" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="79" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="66" spans="1:1" s="82" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="82" t="s">
+    <row r="66" spans="1:1" s="79" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A66" s="79" t="s">
         <v>161</v>
       </c>
     </row>

</xml_diff>

<commit_message>
A whole bunch of little things
</commit_message>
<xml_diff>
--- a/Monopoly Game .xlsx
+++ b/Monopoly Game .xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="28800" windowHeight="16580" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="28800" windowHeight="16580" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Classes" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="167">
   <si>
     <t>Player</t>
   </si>
@@ -147,9 +147,6 @@
   </si>
   <si>
     <t>Utilities</t>
-  </si>
-  <si>
-    <t>Actions</t>
   </si>
   <si>
     <t>Tax</t>
@@ -1488,8 +1485,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M3" sqref="M3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N2" sqref="N2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1539,47 +1536,45 @@
       </c>
       <c r="E2" s="21"/>
       <c r="F2" s="22" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="I2" s="74" t="s">
         <v>10</v>
       </c>
-      <c r="N2" s="74" t="s">
-        <v>39</v>
-      </c>
+      <c r="N2" s="74"/>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A3" s="43"/>
       <c r="B3" s="44"/>
       <c r="C3" s="32" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D3" s="10"/>
       <c r="E3" s="33"/>
       <c r="F3" s="45"/>
       <c r="H3" s="74" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="I3" s="74" t="s">
         <v>38</v>
       </c>
       <c r="L3" s="74" t="s">
+        <v>39</v>
+      </c>
+      <c r="M3" s="74" t="s">
         <v>40</v>
       </c>
-      <c r="M3" s="74" t="s">
-        <v>41</v>
-      </c>
       <c r="N3" t="s">
+        <v>49</v>
+      </c>
+      <c r="O3" t="s">
         <v>50</v>
       </c>
-      <c r="O3" t="s">
+      <c r="P3" t="s">
         <v>51</v>
       </c>
-      <c r="P3" t="s">
+      <c r="Q3" t="s">
         <v>52</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="4" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -1592,16 +1587,16 @@
       <c r="E4" s="27"/>
       <c r="F4" s="28"/>
       <c r="H4" t="s">
+        <v>41</v>
+      </c>
+      <c r="I4" t="s">
         <v>42</v>
       </c>
-      <c r="I4" t="s">
-        <v>43</v>
-      </c>
       <c r="L4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="M4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="5" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -1612,13 +1607,13 @@
       <c r="E5" s="41"/>
       <c r="F5" s="41"/>
       <c r="I5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="L5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="M5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.2">
@@ -1637,7 +1632,7 @@
       </c>
       <c r="F6" s="22"/>
       <c r="I6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.2">
@@ -1862,7 +1857,7 @@
       <c r="B28" s="13"/>
       <c r="C28" s="14"/>
       <c r="D28" s="15" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E28" s="16"/>
       <c r="F28" s="17"/>
@@ -1872,7 +1867,7 @@
       <c r="B29" s="13"/>
       <c r="C29" s="14"/>
       <c r="D29" s="15" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E29" s="16"/>
       <c r="F29" s="17"/>
@@ -1951,7 +1946,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
@@ -1968,25 +1963,25 @@
   <sheetData>
     <row r="1" spans="1:13" s="57" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="86" t="s">
+        <v>57</v>
+      </c>
+      <c r="B1" s="86" t="s">
         <v>58</v>
       </c>
-      <c r="B1" s="86" t="s">
+      <c r="C1" s="86" t="s">
+        <v>83</v>
+      </c>
+      <c r="D1" s="86" t="s">
+        <v>39</v>
+      </c>
+      <c r="E1" s="87" t="s">
         <v>59</v>
       </c>
-      <c r="C1" s="86" t="s">
+      <c r="F1" s="87" t="s">
+        <v>60</v>
+      </c>
+      <c r="G1" s="87" t="s">
         <v>84</v>
-      </c>
-      <c r="D1" s="86" t="s">
-        <v>40</v>
-      </c>
-      <c r="E1" s="87" t="s">
-        <v>60</v>
-      </c>
-      <c r="F1" s="87" t="s">
-        <v>61</v>
-      </c>
-      <c r="G1" s="87" t="s">
-        <v>85</v>
       </c>
       <c r="H1" s="85" t="s">
         <v>12</v>
@@ -2006,27 +2001,27 @@
       <c r="F2" s="87"/>
       <c r="G2" s="87"/>
       <c r="H2" s="58" t="s">
+        <v>85</v>
+      </c>
+      <c r="I2" s="58" t="s">
         <v>86</v>
       </c>
-      <c r="I2" s="58" t="s">
+      <c r="J2" s="58" t="s">
         <v>87</v>
       </c>
-      <c r="J2" s="58" t="s">
+      <c r="K2" s="58" t="s">
         <v>88</v>
       </c>
-      <c r="K2" s="58" t="s">
+      <c r="L2" s="58" t="s">
         <v>89</v>
       </c>
-      <c r="L2" s="58" t="s">
+      <c r="M2" s="58" t="s">
         <v>90</v>
-      </c>
-      <c r="M2" s="58" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" s="47" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C3" s="46">
         <v>0</v>
@@ -2034,7 +2029,7 @@
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" s="75" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B4" s="76">
         <v>1</v>
@@ -2072,7 +2067,7 @@
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" s="69" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C5" s="46">
         <v>2</v>
@@ -2080,7 +2075,7 @@
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6" s="75" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B6" s="76">
         <v>1</v>
@@ -2118,7 +2113,7 @@
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7" s="63" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C7" s="46">
         <v>4</v>
@@ -2126,7 +2121,7 @@
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8" s="56" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C8" s="46">
         <v>5</v>
@@ -2137,7 +2132,7 @@
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9" s="48" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B9" s="64">
         <v>2</v>
@@ -2175,7 +2170,7 @@
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A10" s="69" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C10" s="46">
         <v>7</v>
@@ -2183,7 +2178,7 @@
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A11" s="48" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B11" s="64">
         <v>2</v>
@@ -2221,7 +2216,7 @@
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A12" s="48" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B12" s="64">
         <v>2</v>
@@ -2259,7 +2254,7 @@
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A13" s="47" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C13" s="46">
         <v>10</v>
@@ -2267,7 +2262,7 @@
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A14" s="49" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B14" s="65">
         <v>3</v>
@@ -2305,7 +2300,7 @@
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A15" s="68" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C15" s="46">
         <v>12</v>
@@ -2316,7 +2311,7 @@
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A16" s="49" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B16" s="65">
         <v>3</v>
@@ -2354,7 +2349,7 @@
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A17" s="49" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B17" s="65">
         <v>3</v>
@@ -2392,7 +2387,7 @@
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A18" s="56" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B18" s="61"/>
       <c r="C18" s="61">
@@ -2413,7 +2408,7 @@
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A19" s="50" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B19" s="66">
         <v>4</v>
@@ -2451,7 +2446,7 @@
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A20" s="69" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C20" s="46">
         <v>17</v>
@@ -2459,7 +2454,7 @@
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A21" s="50" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B21" s="66">
         <v>4</v>
@@ -2497,7 +2492,7 @@
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A22" s="50" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B22" s="66">
         <v>4</v>
@@ -2535,7 +2530,7 @@
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A23" s="47" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C23" s="46">
         <v>20</v>
@@ -2543,7 +2538,7 @@
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A24" s="51" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B24" s="67">
         <v>5</v>
@@ -2581,7 +2576,7 @@
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A25" s="69" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C25" s="46">
         <v>22</v>
@@ -2589,7 +2584,7 @@
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A26" s="51" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B26" s="67">
         <v>5</v>
@@ -2627,7 +2622,7 @@
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A27" s="51" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B27" s="67">
         <v>5</v>
@@ -2665,7 +2660,7 @@
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A28" s="56" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C28" s="46">
         <v>25</v>
@@ -2676,7 +2671,7 @@
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A29" s="52" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B29" s="72">
         <v>6</v>
@@ -2714,7 +2709,7 @@
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A30" s="52" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B30" s="72">
         <v>6</v>
@@ -2752,7 +2747,7 @@
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A31" s="68" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C31" s="46">
         <v>28</v>
@@ -2763,7 +2758,7 @@
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A32" s="52" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B32" s="72">
         <v>6</v>
@@ -2801,7 +2796,7 @@
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A33" s="60" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C33" s="46">
         <v>30</v>
@@ -2809,7 +2804,7 @@
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A34" s="53" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B34" s="71">
         <v>7</v>
@@ -2847,7 +2842,7 @@
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A35" s="53" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B35" s="71">
         <v>7</v>
@@ -2885,7 +2880,7 @@
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A36" s="69" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C36" s="46">
         <v>33</v>
@@ -2893,7 +2888,7 @@
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A37" s="53" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B37" s="71">
         <v>7</v>
@@ -2931,7 +2926,7 @@
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A38" s="56" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C38" s="46">
         <v>35</v>
@@ -2942,7 +2937,7 @@
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A39" s="73" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C39" s="46">
         <v>36</v>
@@ -2950,7 +2945,7 @@
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A40" s="54" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B40" s="70">
         <v>8</v>
@@ -2988,7 +2983,7 @@
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A41" s="63" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C41" s="46">
         <v>38</v>
@@ -2996,7 +2991,7 @@
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A42" s="54" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B42" s="70">
         <v>8</v>
@@ -3064,35 +3059,35 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="78" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="77" t="s">
+        <v>107</v>
+      </c>
+      <c r="B2" s="77" t="s">
         <v>108</v>
       </c>
-      <c r="B2" s="77" t="s">
+      <c r="C2" s="77" t="s">
         <v>109</v>
       </c>
-      <c r="C2" s="77" t="s">
+      <c r="D2" s="77" t="s">
         <v>110</v>
       </c>
-      <c r="D2" s="77" t="s">
-        <v>111</v>
-      </c>
       <c r="E2" s="77" t="s">
+        <v>117</v>
+      </c>
+      <c r="F2" s="77" t="s">
         <v>118</v>
       </c>
-      <c r="F2" s="77" t="s">
-        <v>119</v>
-      </c>
       <c r="G2" s="77" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -3109,7 +3104,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B4">
         <v>24</v>
@@ -3126,7 +3121,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B5">
         <v>11</v>
@@ -3143,7 +3138,7 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B6">
         <v>-1</v>
@@ -3163,7 +3158,7 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B7">
         <v>-1</v>
@@ -3180,7 +3175,7 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B8">
         <v>-1</v>
@@ -3200,7 +3195,7 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B9">
         <v>-1</v>
@@ -3218,12 +3213,12 @@
         <v>3</v>
       </c>
       <c r="G9" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B10">
         <v>-1</v>
@@ -3241,12 +3236,12 @@
         <v>4</v>
       </c>
       <c r="G10" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B11">
         <v>-1</v>
@@ -3264,12 +3259,12 @@
         <v>5</v>
       </c>
       <c r="G11" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B12">
         <v>-1</v>
@@ -3286,7 +3281,7 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B13">
         <v>-1</v>
@@ -3304,12 +3299,12 @@
         <v>6</v>
       </c>
       <c r="G13" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B14">
         <v>39</v>
@@ -3326,7 +3321,7 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B15">
         <v>-1</v>
@@ -3344,12 +3339,12 @@
         <v>7</v>
       </c>
       <c r="G15" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B16">
         <v>-1</v>
@@ -3366,35 +3361,35 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" s="78" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" s="77" t="s">
+        <v>107</v>
+      </c>
+      <c r="B20" s="77" t="s">
         <v>108</v>
       </c>
-      <c r="B20" s="77" t="s">
+      <c r="C20" s="77" t="s">
         <v>109</v>
       </c>
-      <c r="C20" s="77" t="s">
+      <c r="D20" s="77" t="s">
         <v>110</v>
       </c>
-      <c r="D20" s="77" t="s">
-        <v>111</v>
-      </c>
       <c r="E20" s="77" t="s">
+        <v>117</v>
+      </c>
+      <c r="F20" s="77" t="s">
         <v>118</v>
       </c>
-      <c r="F20" s="77" t="s">
-        <v>119</v>
-      </c>
       <c r="G20" s="77" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B21">
         <v>0</v>
@@ -3411,7 +3406,7 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B22">
         <v>-1</v>
@@ -3428,7 +3423,7 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B23">
         <v>-1</v>
@@ -3445,7 +3440,7 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B24">
         <v>-1</v>
@@ -3462,7 +3457,7 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B25">
         <v>-1</v>
@@ -3482,7 +3477,7 @@
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B26">
         <v>-1</v>
@@ -3500,12 +3495,12 @@
         <v>2</v>
       </c>
       <c r="G26" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B27">
         <v>-1</v>
@@ -3523,12 +3518,12 @@
         <v>3</v>
       </c>
       <c r="G27" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B28">
         <v>-1</v>
@@ -3545,7 +3540,7 @@
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B29">
         <v>-1</v>
@@ -3562,7 +3557,7 @@
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B30">
         <v>-1</v>
@@ -3580,12 +3575,12 @@
         <v>4</v>
       </c>
       <c r="G30" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B31">
         <v>-1</v>
@@ -3602,7 +3597,7 @@
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B32">
         <v>-1</v>
@@ -3619,7 +3614,7 @@
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B33">
         <v>-1</v>
@@ -3636,7 +3631,7 @@
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B34">
         <v>-1</v>
@@ -3653,7 +3648,7 @@
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B35">
         <v>-1</v>
@@ -3671,12 +3666,12 @@
         <v>5</v>
       </c>
       <c r="G35" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B36">
         <v>-1</v>
@@ -3693,7 +3688,7 @@
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B37">
         <v>-1</v>
@@ -3729,102 +3724,102 @@
   <sheetData>
     <row r="1" spans="1:1" s="79" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="79" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="81" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="7" spans="1:1" s="79" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="79" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" s="82" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="13" spans="1:1" s="79" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="79" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" s="82" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" s="83" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="19" spans="1:1" s="79" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="79" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" s="82" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" s="83" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" s="84" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" s="84" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="31" spans="1:1" s="79" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="79" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" s="82" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="37" spans="1:1" s="79" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="79" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="42" spans="1:1" s="79" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="79" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="48" spans="1:1" s="79" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" s="79" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="54" spans="1:1" s="79" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A54" s="79" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="60" spans="1:1" s="79" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A60" s="79" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="66" spans="1:1" s="79" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A66" s="79" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Worked on what happens during a turn.
Various methods and things related to all of that jazz.
</commit_message>
<xml_diff>
--- a/Monopoly Game .xlsx
+++ b/Monopoly Game .xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="28800" windowHeight="16580" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="28800" windowHeight="16580" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Classes" sheetId="1" r:id="rId1"/>
@@ -1485,8 +1485,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N2" sqref="N2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1946,8 +1946,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M42"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9:A42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>